<commit_message>
New edge weights test sheets
</commit_message>
<xml_diff>
--- a/test-files/graph-tests/all-negative-weights.xlsx
+++ b/test-files/graph-tests/all-negative-weights.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="63">
   <si>
     <t>SystematicName</t>
   </si>
@@ -178,6 +178,48 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>E-14</t>
+  </si>
+  <si>
+    <t>E-1</t>
+  </si>
+  <si>
+    <t>E-2</t>
+  </si>
+  <si>
+    <t>E-3</t>
+  </si>
+  <si>
+    <t>E-4</t>
+  </si>
+  <si>
+    <t>E-5</t>
+  </si>
+  <si>
+    <t>E-6</t>
+  </si>
+  <si>
+    <t>E-7</t>
+  </si>
+  <si>
+    <t>E-8</t>
+  </si>
+  <si>
+    <t>E-9</t>
+  </si>
+  <si>
+    <t>E-10</t>
+  </si>
+  <si>
+    <t>E-11</t>
+  </si>
+  <si>
+    <t>E-12</t>
+  </si>
+  <si>
+    <t>E-13</t>
   </si>
 </sst>
 </file>
@@ -223,8 +265,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,11 +277,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2365,7 +2411,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="B1" sqref="B1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2375,51 +2421,51 @@
         <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="L1" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="N1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="O1" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2466,7 +2512,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>-1</v>
@@ -2513,7 +2559,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2560,7 +2606,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2607,7 +2653,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2654,7 +2700,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2701,7 +2747,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2748,7 +2794,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2795,7 +2841,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2842,7 +2888,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2889,7 +2935,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2936,7 +2982,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2983,7 +3029,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3030,7 +3076,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>0</v>

</xml_diff>